<commit_message>
Made package to hold Heineman's code.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tommy\git\Kabasuji\Kabasuji\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>entity</t>
   </si>
@@ -36,9 +32,6 @@
   </si>
   <si>
     <t>move</t>
-  </si>
-  <si>
-    <t>toBeDeleted</t>
   </si>
   <si>
     <t>view</t>
@@ -367,7 +360,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,22 +432,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="B8" s="2">
         <v>0.122</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Completed Level Testing. Need to check on Release Testing
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Calvin/git/Kabasuji/Kabasuji/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="5910"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="7120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -43,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,19 +364,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1">
         <v>42482</v>
       </c>
@@ -392,56 +399,72 @@
         <v>42488</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0.52700000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>0.33800000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>0.122</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
+      <c r="D8" s="2">
+        <v>0.17100000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed the way a piece looks(added outlines for each tile). Update code coverage sheet. Drag from bullpen still need work on, pieces can only be dragged within the bounds of the bullpen at the moment.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Calvin/git/Kabasuji/Kabasuji/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="7120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -50,7 +46,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -367,16 +363,16 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>42482</v>
       </c>
@@ -399,66 +395,84 @@
         <v>42488</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0.52700000000000002</v>
       </c>
+      <c r="C2" s="2">
+        <v>0.52700000000000002</v>
+      </c>
       <c r="D2" s="2">
         <v>0.33800000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
       <c r="D3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
       </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
       <c r="D5" s="2">
         <v>0.51700000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
       </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
+        <v>0.122</v>
+      </c>
+      <c r="C8" s="2">
         <v>0.122</v>
       </c>
       <c r="D8" s="2">

</xml_diff>

<commit_message>
Added toString overrides to level classes. This will be useful when we need file names when saving the levels.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="5895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="4980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,13 +363,14 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -408,6 +409,9 @@
       <c r="D2" s="2">
         <v>0.33800000000000002</v>
       </c>
+      <c r="E2" s="2">
+        <v>0.70099999999999996</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -422,6 +426,9 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
+      <c r="E3" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -436,6 +443,9 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
+      <c r="E4" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -450,6 +460,9 @@
       <c r="D5" s="2">
         <v>0.51700000000000002</v>
       </c>
+      <c r="E5" s="2">
+        <v>0.17100000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -464,6 +477,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
+      <c r="E6" s="2">
+        <v>0.379</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -477,6 +493,9 @@
       </c>
       <c r="D8" s="2">
         <v>0.17100000000000001</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.17699999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just organizing things to start testing GUI later.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24180" windowHeight="4980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>entity</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>^I feel like this is wrong, but it's what my computer says. -LilyAnne</t>
   </si>
 </sst>
 </file>
@@ -360,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +415,9 @@
       <c r="E2" s="2">
         <v>0.70099999999999996</v>
       </c>
+      <c r="F2" s="2">
+        <v>0.69399999999999995</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -429,6 +435,9 @@
       <c r="E3" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="F3" s="2">
+        <v>0.112</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -446,6 +455,9 @@
       <c r="E4" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="F4" s="2">
+        <v>0.46600000000000003</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -463,6 +475,9 @@
       <c r="E5" s="2">
         <v>0.17100000000000001</v>
       </c>
+      <c r="F5" s="2">
+        <v>0.17199999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -480,6 +495,9 @@
       <c r="E6" s="2">
         <v>0.379</v>
       </c>
+      <c r="F6" s="2">
+        <v>0.39100000000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -496,6 +514,14 @@
       </c>
       <c r="E8" s="2">
         <v>0.17699999999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.44700000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More Test Case Fixes.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>entity</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>total</t>
-  </si>
-  <si>
-    <t>^I feel like this is wrong, but it's what my computer says. -LilyAnne</t>
   </si>
 </sst>
 </file>
@@ -415,9 +412,7 @@
       <c r="E2" s="2">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F2" s="2">
-        <v>0.69399999999999995</v>
-      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -435,9 +430,7 @@
       <c r="E3" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F3" s="2">
-        <v>0.112</v>
-      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -455,9 +448,7 @@
       <c r="E4" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.46600000000000003</v>
-      </c>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -475,9 +466,7 @@
       <c r="E5" s="2">
         <v>0.17100000000000001</v>
       </c>
-      <c r="F5" s="2">
-        <v>0.17199999999999999</v>
-      </c>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -495,9 +484,7 @@
       <c r="E6" s="2">
         <v>0.379</v>
       </c>
-      <c r="F6" s="2">
-        <v>0.39100000000000001</v>
-      </c>
+      <c r="F6" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -515,15 +502,9 @@
       <c r="E8" s="2">
         <v>0.17699999999999999</v>
       </c>
-      <c r="F8" s="2">
-        <v>0.44700000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>6</v>
-      </c>
-    </row>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First GUI test and updated Spreadsheet.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>entity</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>Serializers</t>
   </si>
 </sst>
 </file>
@@ -363,7 +366,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +415,9 @@
       <c r="E2" s="2">
         <v>0.70099999999999996</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>0.61299999999999999</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -430,7 +435,9 @@
       <c r="E3" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>8.6999999999999994E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -448,7 +455,9 @@
       <c r="E4" s="2">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>0.46100000000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -466,7 +475,9 @@
       <c r="E5" s="2">
         <v>0.17100000000000001</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>0.29099999999999998</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -484,27 +495,41 @@
       <c r="E6" s="2">
         <v>0.379</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.3000000000000001E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B9" s="2">
         <v>0.122</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C9" s="2">
         <v>0.122</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="2">
         <v>0.17100000000000001</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="2">
         <v>0.17699999999999999</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25"/>
+      <c r="F9" s="2">
+        <v>0.434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Just more GUI tests.  Board Tests too.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17220" windowHeight="5145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18480" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -366,7 +366,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,6 +374,7 @@
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -418,6 +419,9 @@
       <c r="F2" s="2">
         <v>0.61299999999999999</v>
       </c>
+      <c r="G2" s="2">
+        <v>0.29299999999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -438,6 +442,9 @@
       <c r="F3" s="2">
         <v>8.6999999999999994E-2</v>
       </c>
+      <c r="G3" s="2">
+        <v>9.3000000000000013E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -458,6 +465,9 @@
       <c r="F4" s="2">
         <v>0.46100000000000002</v>
       </c>
+      <c r="G4" s="2">
+        <v>0.89700000000000002</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -478,6 +488,9 @@
       <c r="F5" s="2">
         <v>0.29099999999999998</v>
       </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -498,6 +511,9 @@
       <c r="F6" s="2">
         <v>0.41499999999999998</v>
       </c>
+      <c r="G6" s="2">
+        <v>0.41499999999999998</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -506,6 +522,9 @@
       <c r="F7" s="2">
         <v>1.3000000000000001E-2</v>
       </c>
+      <c r="G7">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F8" s="2"/>
@@ -528,6 +547,9 @@
       </c>
       <c r="F9" s="2">
         <v>0.434</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.66299999999999992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Code Coverage sheet.  Almost at 80% for our current code!
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>0.61299999999999999</v>
       </c>
       <c r="G2" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>0.29099999999999998</v>
       </c>
       <c r="G5" s="2">
-        <v>0</v>
+        <v>0.29099999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -522,8 +522,8 @@
       <c r="F7" s="2">
         <v>1.3000000000000001E-2</v>
       </c>
-      <c r="G7">
-        <v>1.3</v>
+      <c r="G7" s="2">
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>0.434</v>
       </c>
       <c r="G9" s="2">
-        <v>0.66299999999999992</v>
+        <v>0.748</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Code Coverage Spreadsheet
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>0.61299999999999999</v>
       </c>
       <c r="G2" s="2">
-        <v>0.75600000000000001</v>
+        <v>0.79500000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>0.434</v>
       </c>
       <c r="G9" s="2">
-        <v>0.72199999999999998</v>
+        <v>0.72899999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reverted to old way of drawing tiles.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +420,7 @@
         <v>0.61299999999999999</v>
       </c>
       <c r="G2" s="2">
-        <v>0.79500000000000004</v>
+        <v>0.75600000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>0.434</v>
       </c>
       <c r="G9" s="2">
-        <v>0.72899999999999998</v>
+        <v>0.72199999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Did more GUI testing.  Got test coverage back up to 70 percent.
</commit_message>
<xml_diff>
--- a/Kabasuji/DayToDayCodeCoverage.xlsx
+++ b/Kabasuji/DayToDayCodeCoverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15285" windowHeight="5160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,9 +375,10 @@
     <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>42482</v>
       </c>
@@ -402,8 +403,11 @@
       <c r="I1" s="1">
         <v>42490</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1">
+        <v>42430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -431,8 +435,11 @@
       <c r="I2" s="2">
         <v>0.72299999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2">
+        <v>0.72299999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -460,8 +467,11 @@
       <c r="I3" s="2">
         <v>0.107</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -489,8 +499,11 @@
       <c r="I4" s="2">
         <v>0.76400000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2">
+        <v>0.81900000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -518,8 +531,11 @@
       <c r="I5" s="2">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -547,8 +563,11 @@
       <c r="I6" s="2">
         <v>0.47099999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="2">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -564,11 +583,15 @@
       <c r="I7" s="2">
         <v>1.3000000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -595,6 +618,9 @@
       </c>
       <c r="I9" s="2">
         <v>0.626</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.70099999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>